<commit_message>
[Chwthewke.PasswordManager2] PasswordEditor : fix Password generation state transitions
</commit_message>
<xml_diff>
--- a/doc/StateRelationships.xlsx
+++ b/doc/StateRelationships.xlsx
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J7"/>
+  <dimension ref="A2:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,9 +475,8 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="C4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -501,21 +500,21 @@
         <v>1</v>
       </c>
       <c r="B5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
         <f>FALSE</f>
         <v>0</v>
-      </c>
-      <c r="C5" t="b">
-        <f>TRUE</f>
-        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -534,8 +533,8 @@
         <v>1</v>
       </c>
       <c r="C6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -547,38 +546,9 @@
         <v>1</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="B7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>